<commit_message>
Update TCR, starcat, and various smaller changes
</commit_message>
<xml_diff>
--- a/10_Miscellaneous/10.2_Timepoints.xlsx
+++ b/10_Miscellaneous/10.2_Timepoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Partners HealthCare Dropbox/Peter van Galen/Projects/ImmuneEscapeTP53/TP53_ImmuneEscape/10_Miscellaneous/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Partners HealthCare Dropbox/Peter van Galen/Projects/ImmuneEscapeTP53/hsct_immune_reconstitution/10_Miscellaneous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F74F77D-97EE-B748-A045-AB99DD9551EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3079D346-CBAC-BD48-A5E0-4E6686A4D813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A6366E64-3C3B-2243-AB5A-1CC8410567B2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34400" windowHeight="21580" xr2:uid="{A6366E64-3C3B-2243-AB5A-1CC8410567B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="175">
   <si>
     <t>Patient_id</t>
   </si>
@@ -134,12 +134,6 @@
     <t>P23</t>
   </si>
   <si>
-    <t>P20_rel</t>
-  </si>
-  <si>
-    <t>P23_rel</t>
-  </si>
-  <si>
     <t>P24</t>
   </si>
   <si>
@@ -158,9 +152,6 @@
     <t>P29</t>
   </si>
   <si>
-    <t>P29_rel</t>
-  </si>
-  <si>
     <t>P30</t>
   </si>
   <si>
@@ -173,30 +164,6 @@
     <t>P33</t>
   </si>
   <si>
-    <t>P31_rel</t>
-  </si>
-  <si>
-    <t>P30_rel</t>
-  </si>
-  <si>
-    <t>P24_rel</t>
-  </si>
-  <si>
-    <t>P25_rel</t>
-  </si>
-  <si>
-    <t>P27_rel</t>
-  </si>
-  <si>
-    <t>P33_rel</t>
-  </si>
-  <si>
-    <t>P32_rel</t>
-  </si>
-  <si>
-    <t>P28_rel</t>
-  </si>
-  <si>
     <t>Sample_type</t>
   </si>
   <si>
@@ -227,12 +194,6 @@
     <t>Death</t>
   </si>
   <si>
-    <t>P21_rel</t>
-  </si>
-  <si>
-    <t>P22_rel</t>
-  </si>
-  <si>
     <t>P01_Rem1</t>
   </si>
   <si>
@@ -558,6 +519,48 @@
   </si>
   <si>
     <t>P33_Tx</t>
+  </si>
+  <si>
+    <t>P27_Rel</t>
+  </si>
+  <si>
+    <t>P28_Rel</t>
+  </si>
+  <si>
+    <t>P29_Rel</t>
+  </si>
+  <si>
+    <t>P30_Rel</t>
+  </si>
+  <si>
+    <t>P31_Rel</t>
+  </si>
+  <si>
+    <t>P32_Rel</t>
+  </si>
+  <si>
+    <t>P33_Rel</t>
+  </si>
+  <si>
+    <t>P20_Rel</t>
+  </si>
+  <si>
+    <t>P21_Rel</t>
+  </si>
+  <si>
+    <t>P22_Rel</t>
+  </si>
+  <si>
+    <t>P23_Rel</t>
+  </si>
+  <si>
+    <t>P24_Rel</t>
+  </si>
+  <si>
+    <t>P25_Rel</t>
+  </si>
+  <si>
+    <t>P26_Rel</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11086070-A44B-7A4A-BB47-98F55A4430A5}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J87" sqref="J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,13 +1038,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1055,16 +1058,16 @@
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1078,16 +1081,16 @@
         <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1101,16 +1104,16 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2">
         <v>97</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1124,16 +1127,16 @@
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2">
         <v>181</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1147,17 +1150,17 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F6" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1171,16 +1174,16 @@
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1194,16 +1197,16 @@
         <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1217,16 +1220,16 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F9" s="2">
         <v>168</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1240,16 +1243,16 @@
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2">
         <v>798</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1263,16 +1266,16 @@
         <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F11" s="4">
         <v>1726</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1286,16 +1289,16 @@
         <v>18</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1309,16 +1312,16 @@
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F13" s="2">
         <v>365</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1332,16 +1335,16 @@
         <v>18</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F14" s="4">
         <v>1297</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1355,16 +1358,16 @@
         <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1378,16 +1381,16 @@
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F16" s="2">
         <v>96</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1401,17 +1404,17 @@
         <v>18</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F17" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1425,16 +1428,16 @@
         <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F18" s="3">
         <v>0</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1448,16 +1451,16 @@
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F19" s="2">
         <v>90</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1471,17 +1474,17 @@
         <v>18</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F20" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1495,16 +1498,16 @@
         <v>18</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F21" s="3">
         <v>0</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1518,16 +1521,16 @@
         <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F22" s="2">
         <v>114</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1541,17 +1544,17 @@
         <v>18</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F23" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1565,16 +1568,16 @@
         <v>27</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F24" s="3">
         <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1588,16 +1591,16 @@
         <v>27</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F25" s="2">
         <v>104</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1611,17 +1614,17 @@
         <v>27</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F26" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1635,16 +1638,16 @@
         <v>27</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1658,16 +1661,16 @@
         <v>27</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F28" s="2">
         <v>118</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1681,17 +1684,17 @@
         <v>27</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F29" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1705,16 +1708,16 @@
         <v>27</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F30" s="3">
         <v>0</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1728,16 +1731,16 @@
         <v>27</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F31" s="2">
         <v>68</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1751,17 +1754,17 @@
         <v>27</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F32" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1775,16 +1778,16 @@
         <v>27</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F33" s="3">
         <v>0</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1798,16 +1801,16 @@
         <v>27</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F34" s="2">
         <v>81</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1821,17 +1824,17 @@
         <v>27</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F35" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1845,16 +1848,16 @@
         <v>27</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F36" s="3">
         <v>0</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1868,16 +1871,16 @@
         <v>27</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F37" s="2">
         <v>97</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1891,17 +1894,17 @@
         <v>27</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F38" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1915,16 +1918,16 @@
         <v>27</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F39" s="3">
         <v>0</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1938,16 +1941,16 @@
         <v>27</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F40" s="2">
         <v>99</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1961,17 +1964,17 @@
         <v>27</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F41" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1985,16 +1988,16 @@
         <v>27</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F42" s="3">
         <v>0</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2008,16 +2011,16 @@
         <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F43" s="2">
         <v>97</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2031,17 +2034,17 @@
         <v>27</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F44" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2055,16 +2058,16 @@
         <v>27</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F45" s="3">
         <v>0</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2078,16 +2081,16 @@
         <v>27</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F46" s="2">
         <v>98</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2101,17 +2104,17 @@
         <v>27</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F47" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2125,16 +2128,16 @@
         <v>27</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F48" s="3">
         <v>0</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -2148,16 +2151,16 @@
         <v>27</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F49" s="2">
         <v>147</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2171,17 +2174,17 @@
         <v>27</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F50" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2195,16 +2198,16 @@
         <v>27</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F51" s="3">
         <v>0</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -2218,16 +2221,16 @@
         <v>27</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F52" s="2">
         <v>98</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -2241,17 +2244,17 @@
         <v>27</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F53" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -2265,16 +2268,16 @@
         <v>27</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F54" s="3">
         <v>0</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -2288,16 +2291,16 @@
         <v>27</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F55" s="2">
         <v>116</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -2311,16 +2314,16 @@
         <v>27</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F56" s="4">
         <v>252</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -2334,16 +2337,16 @@
         <v>27</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F57" s="3">
         <v>0</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -2357,16 +2360,16 @@
         <v>27</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F58" s="2">
         <v>89</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -2380,17 +2383,17 @@
         <v>27</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F59" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2404,16 +2407,16 @@
         <v>27</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F60" s="3">
         <v>0</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -2427,16 +2430,16 @@
         <v>27</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F61" s="2">
         <v>104</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2450,17 +2453,17 @@
         <v>27</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F62" s="4">
         <f>42*30.44</f>
         <v>1278.48</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -2474,16 +2477,16 @@
         <v>18</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2497,16 +2500,16 @@
         <v>18</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F64" s="3">
         <v>0</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -2520,16 +2523,16 @@
         <v>18</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F65" s="2">
         <v>104</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -2543,7 +2546,7 @@
         <v>18</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>19</v>
@@ -2552,7 +2555,7 @@
         <v>188</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -2566,7 +2569,7 @@
         <v>18</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>19</v>
@@ -2575,7 +2578,7 @@
         <v>294</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -2589,16 +2592,16 @@
         <v>18</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F68" s="4">
         <v>369</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -2612,16 +2615,16 @@
         <v>18</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2635,16 +2638,16 @@
         <v>18</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F70" s="3">
         <v>0</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2658,16 +2661,16 @@
         <v>18</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F71" s="2">
         <v>90</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -2681,7 +2684,7 @@
         <v>18</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="E72" s="9" t="s">
         <v>19</v>
@@ -2690,7 +2693,7 @@
         <v>502</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2704,16 +2707,16 @@
         <v>18</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F73" s="4">
         <v>579</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2727,16 +2730,16 @@
         <v>18</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F74" s="3">
         <v>0</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2750,16 +2753,16 @@
         <v>18</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F75" s="2">
         <v>110</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2773,7 +2776,7 @@
         <v>18</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="E76" s="9" t="s">
         <v>19</v>
@@ -2782,7 +2785,7 @@
         <v>166</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2796,16 +2799,16 @@
         <v>18</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F77" s="4">
         <v>226</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2819,16 +2822,16 @@
         <v>18</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2842,16 +2845,16 @@
         <v>18</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F79" s="3">
         <v>0</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2865,16 +2868,16 @@
         <v>18</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F80" s="2">
         <v>116</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2888,16 +2891,16 @@
         <v>18</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F81" s="2">
         <v>377</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2911,7 +2914,7 @@
         <v>18</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>19</v>
@@ -2920,7 +2923,7 @@
         <v>1201</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -2934,21 +2937,21 @@
         <v>18</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F83" s="6">
         <v>1283</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>19</v>
@@ -2957,21 +2960,21 @@
         <v>27</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F84" s="3">
         <v>0</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>19</v>
@@ -2980,21 +2983,21 @@
         <v>27</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F85" s="2">
         <v>88</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>19</v>
@@ -3003,7 +3006,7 @@
         <v>27</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>19</v>
@@ -3012,12 +3015,12 @@
         <v>168</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>19</v>
@@ -3026,21 +3029,21 @@
         <v>27</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F87" s="6">
         <v>423</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>19</v>
@@ -3049,21 +3052,21 @@
         <v>27</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F88" s="3">
         <v>0</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>19</v>
@@ -3072,21 +3075,21 @@
         <v>27</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F89" s="2">
         <v>104</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B90" s="9" t="s">
         <v>19</v>
@@ -3095,7 +3098,7 @@
         <v>27</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>48</v>
+        <v>173</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>19</v>
@@ -3104,12 +3107,12 @@
         <v>522</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>19</v>
@@ -3118,21 +3121,21 @@
         <v>27</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F91" s="6">
         <v>1882</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>19</v>
@@ -3141,21 +3144,21 @@
         <v>27</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F92" s="3">
         <v>0</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>19</v>
@@ -3164,21 +3167,21 @@
         <v>27</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F93" s="2">
         <v>104</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>19</v>
@@ -3187,7 +3190,7 @@
         <v>27</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>93</v>
+        <v>174</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>19</v>
@@ -3196,12 +3199,12 @@
         <v>133</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>19</v>
@@ -3210,21 +3213,21 @@
         <v>27</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F95" s="4">
         <v>774</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>19</v>
@@ -3233,21 +3236,21 @@
         <v>27</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F96" s="3">
         <v>0</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>19</v>
@@ -3256,21 +3259,21 @@
         <v>27</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F97" s="2">
         <v>83</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B98" s="9" t="s">
         <v>19</v>
@@ -3279,7 +3282,7 @@
         <v>27</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>19</v>
@@ -3288,12 +3291,12 @@
         <v>146</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>19</v>
@@ -3302,21 +3305,21 @@
         <v>27</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F99" s="6">
         <v>240</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>19</v>
@@ -3325,21 +3328,21 @@
         <v>27</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F100" s="3">
         <v>0</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>19</v>
@@ -3348,7 +3351,7 @@
         <v>27</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>19</v>
@@ -3357,12 +3360,12 @@
         <v>93</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>19</v>
@@ -3371,21 +3374,21 @@
         <v>27</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F102" s="4">
         <v>133</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>19</v>
@@ -3394,21 +3397,21 @@
         <v>27</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F103" s="3">
         <v>0</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>19</v>
@@ -3417,7 +3420,7 @@
         <v>27</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="E104" s="9" t="s">
         <v>19</v>
@@ -3426,12 +3429,12 @@
         <v>61</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>19</v>
@@ -3440,7 +3443,7 @@
         <v>27</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="E105" s="7" t="s">
         <v>19</v>
@@ -3449,12 +3452,12 @@
         <v>90</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>19</v>
@@ -3463,21 +3466,21 @@
         <v>27</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F106" s="4">
         <v>122</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>17</v>
@@ -3486,21 +3489,21 @@
         <v>18</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>17</v>
@@ -3509,21 +3512,21 @@
         <v>18</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F108" s="3">
         <v>0</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>17</v>
@@ -3532,21 +3535,21 @@
         <v>18</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F109" s="2">
         <v>34</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>17</v>
@@ -3555,7 +3558,7 @@
         <v>18</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>46</v>
+        <v>164</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>19</v>
@@ -3564,12 +3567,12 @@
         <v>104</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>17</v>
@@ -3578,21 +3581,21 @@
         <v>18</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F111" s="4">
         <v>544</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>17</v>
@@ -3601,21 +3604,21 @@
         <v>18</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>17</v>
@@ -3624,21 +3627,21 @@
         <v>18</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F113" s="3">
         <v>0</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>17</v>
@@ -3647,21 +3650,21 @@
         <v>18</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F114" s="2">
         <v>47</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B115" s="9" t="s">
         <v>17</v>
@@ -3670,7 +3673,7 @@
         <v>18</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="E115" s="9" t="s">
         <v>19</v>
@@ -3679,12 +3682,12 @@
         <v>79</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>17</v>
@@ -3693,7 +3696,7 @@
         <v>18</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="E116" s="7" t="s">
         <v>19</v>
@@ -3702,12 +3705,12 @@
         <v>93</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>17</v>
@@ -3716,21 +3719,21 @@
         <v>18</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F117" s="4">
         <v>162</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>17</v>
@@ -3739,21 +3742,21 @@
         <v>18</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>17</v>
@@ -3762,21 +3765,21 @@
         <v>18</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F119" s="3">
         <v>0</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>17</v>
@@ -3785,21 +3788,21 @@
         <v>18</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F120" s="2">
         <v>35</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B121" s="9" t="s">
         <v>17</v>
@@ -3808,7 +3811,7 @@
         <v>18</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>19</v>
@@ -3817,12 +3820,12 @@
         <v>70</v>
       </c>
       <c r="G121" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="122" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>17</v>
@@ -3831,21 +3834,21 @@
         <v>18</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F122" s="6">
         <v>151</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>17</v>
@@ -3854,21 +3857,21 @@
         <v>18</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>17</v>
@@ -3877,21 +3880,21 @@
         <v>18</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F124" s="3">
         <v>0</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>17</v>
@@ -3900,21 +3903,21 @@
         <v>18</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F125" s="2">
         <v>33</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B126" s="9" t="s">
         <v>17</v>
@@ -3923,7 +3926,7 @@
         <v>18</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>50</v>
+        <v>167</v>
       </c>
       <c r="E126" s="9" t="s">
         <v>19</v>
@@ -3932,12 +3935,12 @@
         <v>258</v>
       </c>
       <c r="G126" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>17</v>
@@ -3946,16 +3949,16 @@
         <v>18</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F127" s="4">
         <v>346</v>
       </c>
       <c r="G127" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final updates before submission: README, various small fixes
</commit_message>
<xml_diff>
--- a/10_Miscellaneous/10.2_Timepoints.xlsx
+++ b/10_Miscellaneous/10.2_Timepoints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Partners HealthCare Dropbox/Peter van Galen/Projects/ImmuneEscapeTP53/hsct_immune_reconstitution/10_Miscellaneous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3079D346-CBAC-BD48-A5E0-4E6686A4D813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D88A11D-1A20-2E44-8F00-0DE833ECC78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34400" windowHeight="21580" xr2:uid="{A6366E64-3C3B-2243-AB5A-1CC8410567B2}"/>
   </bookViews>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11086070-A44B-7A4A-BB47-98F55A4430A5}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J87" sqref="J87"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,8 +1156,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>386</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>48</v>
@@ -1410,8 +1409,7 @@
         <v>50</v>
       </c>
       <c r="F17" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>365</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>48</v>
@@ -1480,8 +1478,7 @@
         <v>50</v>
       </c>
       <c r="F20" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>2449</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>48</v>
@@ -1550,8 +1547,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>903</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>48</v>
@@ -1620,8 +1616,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>2534</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>48</v>
@@ -1690,8 +1685,7 @@
         <v>50</v>
       </c>
       <c r="F29" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>2197</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>48</v>
@@ -1760,8 +1754,7 @@
         <v>50</v>
       </c>
       <c r="F32" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>1567</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>48</v>
@@ -1830,8 +1823,7 @@
         <v>50</v>
       </c>
       <c r="F35" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>2205</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>48</v>
@@ -1900,8 +1892,7 @@
         <v>50</v>
       </c>
       <c r="F38" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>1048</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>48</v>
@@ -1970,8 +1961,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>1138</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>48</v>
@@ -2040,8 +2030,7 @@
         <v>50</v>
       </c>
       <c r="F44" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>945</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>48</v>
@@ -2110,8 +2099,7 @@
         <v>50</v>
       </c>
       <c r="F47" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>754</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>48</v>
@@ -2180,8 +2168,7 @@
         <v>50</v>
       </c>
       <c r="F50" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>2345</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>48</v>
@@ -2250,8 +2237,7 @@
         <v>50</v>
       </c>
       <c r="F53" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>1099</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>48</v>
@@ -2389,8 +2375,7 @@
         <v>50</v>
       </c>
       <c r="F59" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>880</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>48</v>
@@ -2459,8 +2444,7 @@
         <v>50</v>
       </c>
       <c r="F62" s="4">
-        <f>42*30.44</f>
-        <v>1278.48</v>
+        <v>951</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>48</v>

</xml_diff>